<commit_message>
LyM me va a matar
</commit_message>
<xml_diff>
--- a/Tarea 2-202420.xlsx
+++ b/Tarea 2-202420.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/lj_sanchezd_uniandes_edu_co/Documents/IIND 4101 - Optimización Avanzada/2024-20/Tareas/Tarea 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/w_bayona_uniandes_edu_co/Documents/College/8. Eighth Semester Stuff/Opti Avanzada IIND4101/Tarea2-IIND4101/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92D6A5F7-5351-42BE-BE8A-8F75447930BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{92D6A5F7-5351-42BE-BE8A-8F75447930BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A97A435-492D-4FA7-98FA-4802B263994C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{81650E00-C281-45CE-979D-E64548F31258}"/>
+    <workbookView minimized="1" xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" xr2:uid="{81650E00-C281-45CE-979D-E64548F31258}"/>
   </bookViews>
   <sheets>
     <sheet name="Opti-drones" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v5.0" hidden="1">'Opti-drones'!$A$1</definedName>
+    <definedName name="_xlchart.v5.1" hidden="1">'Opti-drones'!$A$2:$A$27</definedName>
+    <definedName name="_xlchart.v5.10" hidden="1">'Opti-drones'!$C$1</definedName>
+    <definedName name="_xlchart.v5.11" hidden="1">'Opti-drones'!$C$2:$C$27</definedName>
+    <definedName name="_xlchart.v5.2" hidden="1">'Opti-drones'!$B$1</definedName>
+    <definedName name="_xlchart.v5.3" hidden="1">'Opti-drones'!$B$2:$B$27</definedName>
+    <definedName name="_xlchart.v5.4" hidden="1">'Opti-drones'!$C$1</definedName>
+    <definedName name="_xlchart.v5.5" hidden="1">'Opti-drones'!$C$2:$C$27</definedName>
+    <definedName name="_xlchart.v5.6" hidden="1">'Opti-drones'!$A$1</definedName>
+    <definedName name="_xlchart.v5.7" hidden="1">'Opti-drones'!$A$2:$A$27</definedName>
+    <definedName name="_xlchart.v5.8" hidden="1">'Opti-drones'!$B$1</definedName>
+    <definedName name="_xlchart.v5.9" hidden="1">'Opti-drones'!$B$2:$B$27</definedName>
+  </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -201,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,9 +232,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,7 +254,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -559,463 +570,463 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E163499-7C0C-462B-95B9-4932265BB4E0}">
-  <dimension ref="A2:G34"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4">
+        <v>40</v>
+      </c>
+      <c r="C2" s="4">
+        <v>80</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D3" s="5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D4" s="5">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4">
         <v>8</v>
       </c>
       <c r="C5" s="4">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D5" s="5">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="D7" s="5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4">
+        <v>60</v>
+      </c>
+      <c r="D8" s="5">
         <v>75</v>
-      </c>
-      <c r="D8" s="5">
-        <v>15</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4">
+        <v>77</v>
+      </c>
+      <c r="D9" s="5">
         <v>60</v>
-      </c>
-      <c r="D9" s="5">
-        <v>75</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4">
+        <v>64</v>
+      </c>
+      <c r="D10" s="5">
+        <v>40</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4">
+        <v>75</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="4">
         <v>11</v>
       </c>
-      <c r="B10" s="4">
+      <c r="C12" s="4">
+        <v>84</v>
+      </c>
+      <c r="D12" s="5">
+        <v>70</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4">
+      <c r="B13" s="4">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4">
+        <v>66</v>
+      </c>
+      <c r="D13" s="5">
+        <v>55</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4">
+        <v>51</v>
+      </c>
+      <c r="D14" s="5">
+        <v>40</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4">
+        <v>45</v>
+      </c>
+      <c r="C15" s="4">
+        <v>82</v>
+      </c>
+      <c r="D15" s="5">
+        <v>75</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4">
+        <v>52</v>
+      </c>
+      <c r="D16" s="5">
+        <v>70</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="4">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <v>71</v>
+      </c>
+      <c r="D17" s="5">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4">
+        <v>6</v>
+      </c>
+      <c r="C18" s="4">
+        <v>68</v>
+      </c>
+      <c r="D18" s="5">
+        <v>30</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="4">
+        <v>45</v>
+      </c>
+      <c r="C19" s="4">
+        <v>55</v>
+      </c>
+      <c r="D19" s="5">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="4">
+        <v>39</v>
+      </c>
+      <c r="C20" s="4">
+        <v>85</v>
+      </c>
+      <c r="D20" s="5">
+        <v>90</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="4">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4">
         <v>77</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D21" s="5">
+        <v>30</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4">
+        <v>22</v>
+      </c>
+      <c r="C22" s="4">
+        <v>85</v>
+      </c>
+      <c r="D22" s="5">
+        <v>55</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="4">
+        <v>12</v>
+      </c>
+      <c r="C23" s="4">
+        <v>50</v>
+      </c>
+      <c r="D23" s="5">
         <v>60</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="4">
+        <v>26</v>
+      </c>
+      <c r="C24" s="4">
+        <v>77</v>
+      </c>
+      <c r="D24" s="5">
+        <v>85</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="4">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4">
+        <v>50</v>
+      </c>
+      <c r="D25" s="5">
+        <v>40</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="4">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4">
+        <v>85</v>
+      </c>
+      <c r="D26" s="5">
+        <v>15</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="6">
         <v>12</v>
       </c>
-      <c r="B11" s="4">
-        <v>29</v>
-      </c>
-      <c r="C11" s="4">
-        <v>64</v>
-      </c>
-      <c r="D11" s="5">
-        <v>40</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4">
-        <v>30</v>
-      </c>
-      <c r="C12" s="4">
-        <v>75</v>
-      </c>
-      <c r="D12" s="5">
-        <v>45</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="4">
-        <v>11</v>
-      </c>
-      <c r="C13" s="4">
-        <v>84</v>
-      </c>
-      <c r="D13" s="5">
-        <v>70</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="4">
-        <v>35</v>
-      </c>
-      <c r="C14" s="4">
-        <v>66</v>
-      </c>
-      <c r="D14" s="5">
-        <v>55</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4">
-        <v>27</v>
-      </c>
-      <c r="C15" s="4">
-        <v>51</v>
-      </c>
-      <c r="D15" s="5">
-        <v>40</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="4">
-        <v>45</v>
-      </c>
-      <c r="C16" s="4">
-        <v>82</v>
-      </c>
-      <c r="D16" s="5">
-        <v>75</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="4">
+      <c r="C27" s="6">
+        <v>71</v>
+      </c>
+      <c r="D27" s="7">
         <v>25</v>
       </c>
-      <c r="C17" s="4">
-        <v>52</v>
-      </c>
-      <c r="D17" s="5">
-        <v>70</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="4">
-        <v>15</v>
-      </c>
-      <c r="C18" s="4">
-        <v>71</v>
-      </c>
-      <c r="D18" s="5">
-        <v>15</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="4">
-        <v>6</v>
-      </c>
-      <c r="C19" s="4">
-        <v>68</v>
-      </c>
-      <c r="D19" s="5">
-        <v>30</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="4">
-        <v>45</v>
-      </c>
-      <c r="C20" s="4">
-        <v>55</v>
-      </c>
-      <c r="D20" s="5">
-        <v>10</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="4">
-        <v>39</v>
-      </c>
-      <c r="C21" s="4">
-        <v>85</v>
-      </c>
-      <c r="D21" s="5">
-        <v>90</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="4">
-        <v>9</v>
-      </c>
-      <c r="C22" s="4">
-        <v>77</v>
-      </c>
-      <c r="D22" s="5">
-        <v>30</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="4">
-        <v>22</v>
-      </c>
-      <c r="C23" s="4">
-        <v>85</v>
-      </c>
-      <c r="D23" s="5">
-        <v>55</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="4">
-        <v>12</v>
-      </c>
-      <c r="C24" s="4">
-        <v>50</v>
-      </c>
-      <c r="D24" s="5">
-        <v>60</v>
-      </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="4">
-        <v>26</v>
-      </c>
-      <c r="C25" s="4">
-        <v>77</v>
-      </c>
-      <c r="D25" s="5">
-        <v>85</v>
-      </c>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="4">
-        <v>11</v>
-      </c>
-      <c r="C26" s="4">
-        <v>50</v>
-      </c>
-      <c r="D26" s="5">
-        <v>40</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="4">
-        <v>27</v>
-      </c>
-      <c r="C27" s="4">
-        <v>85</v>
-      </c>
-      <c r="D27" s="5">
-        <v>15</v>
-      </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="6">
-        <v>12</v>
-      </c>
-      <c r="C28" s="6">
-        <v>71</v>
-      </c>
-      <c r="D28" s="8">
-        <v>25</v>
-      </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>